<commit_message>
v3 BOM. cambios para seti
Columna de cambios.
</commit_message>
<xml_diff>
--- a/02.Hardware/MK2 2040/01.EDCPSU/BOM/EDCPSU_MK2_RP2040_BOM-SETI.xlsx
+++ b/02.Hardware/MK2 2040/01.EDCPSU/BOM/EDCPSU_MK2_RP2040_BOM-SETI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Team Dropbox\JRODRIGUEZ\Repositorios\07.MK2\02.Hardware\MK2 2040\01.EDCPSU\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CD642B-8A4B-4E16-9F4A-3B8DED4E48A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C268A14E-EFDB-49E2-96EC-74BFC4184671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EDCPSUMK2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="252">
   <si>
     <t>Qty</t>
   </si>
@@ -372,9 +372,6 @@
     <t>U10</t>
   </si>
   <si>
-    <t>BOM VERSION v1</t>
-  </si>
-  <si>
     <t>MK2-RP2040</t>
   </si>
   <si>
@@ -708,9 +705,6 @@
     <t>Creacion</t>
   </si>
   <si>
-    <t>Suministrado</t>
-  </si>
-  <si>
     <t>0.025R / 1W</t>
   </si>
   <si>
@@ -774,14 +768,35 @@
     <t>R11</t>
   </si>
   <si>
+    <t>Cambios</t>
+  </si>
+  <si>
+    <t>Eliminada</t>
+  </si>
+  <si>
+    <t>Nueva</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
     <t>Se añade el pos 79 con el part R15
-Se añade la pos  con el part D3 con el valor N.C
+Se añade la pos 80 con el part D3 con el valor N.C
 Se añade a la pos 43 el part 57 aumentando su Qty.
 Se cambia el value de la pos 76  a LM4040C30FTA
 Se cambia el valor de la pos 39 part R12 a 0,025mOhm
-Se aumenta la pos 42 con el part R41 
+Se aumenta la pos 46 con el part R41 
 Se aumenta la pos 45 con el part R43 
 Se añade la pos 81 cambia el valor de R11 a 15K</t>
+  </si>
+  <si>
+    <t>Se añade la columna de Cambios</t>
+  </si>
+  <si>
+    <t>BOM VERSION v3</t>
   </si>
 </sst>
 </file>
@@ -1698,7 +1713,7 @@
     <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1795,9 +1810,6 @@
     <xf numFmtId="49" fontId="17" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="47" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1864,9 +1876,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1874,6 +1883,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="45" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="41" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="85">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1962,7 +1974,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Total 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="21">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2075,6 +2087,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2085,11 +2107,51 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2461,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N84"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2484,21 +2546,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.2">
-      <c r="H1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="E2" s="5">
+        <v>45020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="H2" s="5">
-        <v>45020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
@@ -2509,7 +2571,7 @@
         <v>85</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>93</v>
@@ -2571,16 +2633,16 @@
         <v>87</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I7" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="48"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="46"/>
+      <c r="M7" s="46"/>
+      <c r="N7" s="46"/>
     </row>
     <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
@@ -2599,10 +2661,10 @@
         <v>42</v>
       </c>
       <c r="F8" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="34" t="s">
         <v>114</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>115</v>
       </c>
       <c r="H8" s="34">
         <v>1210</v>
@@ -2610,15 +2672,15 @@
       <c r="I8" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="48"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>86</v>
+      <c r="A9" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>82</v>
@@ -2630,7 +2692,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>72</v>
@@ -2644,11 +2706,11 @@
       <c r="I9" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="49"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="47"/>
-      <c r="N9" s="47"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
     </row>
     <row r="10" spans="1:14" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
@@ -2664,10 +2726,10 @@
         <v>34</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" s="34" t="s">
         <v>18</v>
@@ -2678,11 +2740,11 @@
       <c r="I10" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="49"/>
-      <c r="K10" s="47"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
@@ -2698,13 +2760,13 @@
         <v>4</v>
       </c>
       <c r="E11" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="34" t="s">
-        <v>119</v>
-      </c>
       <c r="G11" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H11" s="34">
         <v>1206</v>
@@ -2712,11 +2774,11 @@
       <c r="I11" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="49"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="46"/>
+      <c r="M11" s="46"/>
+      <c r="N11" s="46"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
@@ -2732,10 +2794,10 @@
         <v>2</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="34" t="s">
         <v>18</v>
@@ -2746,11 +2808,11 @@
       <c r="I12" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="49"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="47"/>
-      <c r="M12" s="47"/>
-      <c r="N12" s="47"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="46"/>
+      <c r="L12" s="46"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
@@ -2766,10 +2828,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="34" t="s">
         <v>121</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>122</v>
       </c>
       <c r="G13" s="34" t="s">
         <v>18</v>
@@ -2780,11 +2842,11 @@
       <c r="I13" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
@@ -2802,8 +2864,8 @@
       <c r="E14" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="36" t="s">
-        <v>123</v>
+      <c r="F14" s="34" t="s">
+        <v>122</v>
       </c>
       <c r="G14" s="34" t="s">
         <v>18</v>
@@ -2814,11 +2876,11 @@
       <c r="I14" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="49"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="46"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
@@ -2836,8 +2898,8 @@
       <c r="E15" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="36" t="s">
-        <v>124</v>
+      <c r="F15" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="G15" s="34" t="s">
         <v>18</v>
@@ -2848,11 +2910,11 @@
       <c r="I15" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="49"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="47"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="46"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
@@ -2871,10 +2933,10 @@
         <v>34</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H16" s="34">
         <v>1210</v>
@@ -2882,11 +2944,11 @@
       <c r="I16" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
+      <c r="N16" s="46"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
@@ -2902,10 +2964,10 @@
         <v>1</v>
       </c>
       <c r="E17" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="34" t="s">
         <v>125</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>126</v>
       </c>
       <c r="G17" s="34" t="s">
         <v>18</v>
@@ -2916,11 +2978,11 @@
       <c r="I17" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J17" s="49"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
@@ -2936,10 +2998,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" s="34" t="s">
         <v>127</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>128</v>
       </c>
       <c r="G18" s="34" t="s">
         <v>18</v>
@@ -2950,11 +3012,11 @@
       <c r="I18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="49"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
@@ -2970,10 +3032,10 @@
         <v>2</v>
       </c>
       <c r="E19" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="F19" s="34" t="s">
         <v>129</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>130</v>
       </c>
       <c r="G19" s="34" t="s">
         <v>18</v>
@@ -2984,11 +3046,11 @@
       <c r="I19" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="49"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="N19" s="47"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
@@ -3004,10 +3066,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="34" t="s">
         <v>131</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>132</v>
       </c>
       <c r="G20" s="34" t="s">
         <v>18</v>
@@ -3018,18 +3080,18 @@
       <c r="I20" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="49"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>86</v>
+      <c r="B21" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C21" s="23">
         <v>16</v>
@@ -3041,22 +3103,22 @@
         <v>60</v>
       </c>
       <c r="F21" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="G21" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H21" s="34" t="s">
+      <c r="I21" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="I21" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="J21" s="49"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
-      <c r="N21" s="47"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
@@ -3072,7 +3134,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>56</v>
@@ -3086,18 +3148,18 @@
       <c r="I22" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="J22" s="49"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
-      <c r="N22" s="47"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="46"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>86</v>
+      <c r="B23" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C23" s="23">
         <v>18</v>
@@ -3109,29 +3171,29 @@
         <v>94</v>
       </c>
       <c r="F23" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="H23" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="G23" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="H23" s="34" t="s">
+      <c r="I23" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="I23" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="J23" s="49"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>86</v>
+      <c r="B24" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C24" s="23">
         <v>19</v>
@@ -3140,25 +3202,25 @@
         <v>1</v>
       </c>
       <c r="E24" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="F24" s="34" t="s">
+      <c r="G24" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="G24" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="H24" s="34" t="s">
+      <c r="I24" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="I24" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="J24" s="49"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
-      <c r="N24" s="47"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
@@ -3177,20 +3239,20 @@
         <v>102</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H25" s="34" t="s">
         <v>59</v>
       </c>
       <c r="I25" s="34"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="47"/>
-      <c r="L25" s="47"/>
-      <c r="M25" s="47"/>
-      <c r="N25" s="47"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
@@ -3212,26 +3274,26 @@
         <v>73</v>
       </c>
       <c r="G26" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="H26" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="I26" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="I26" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="J26" s="49"/>
-      <c r="K26" s="47"/>
-      <c r="L26" s="47"/>
-      <c r="M26" s="47"/>
-      <c r="N26" s="47"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="46"/>
+      <c r="N26" s="46"/>
     </row>
     <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>86</v>
+      <c r="B27" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C27" s="23">
         <v>22</v>
@@ -3240,25 +3302,25 @@
         <v>1</v>
       </c>
       <c r="E27" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="G27" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="H27" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="G27" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="H27" s="34" t="s">
+      <c r="I27" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="I27" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="J27" s="50"/>
-      <c r="K27" s="47"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
     </row>
     <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
@@ -3286,13 +3348,13 @@
         <v>105</v>
       </c>
       <c r="I28" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="J28" s="50"/>
-      <c r="K28" s="47"/>
-      <c r="L28" s="47"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
+        <v>152</v>
+      </c>
+      <c r="J28" s="49"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
     </row>
     <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
@@ -3320,18 +3382,18 @@
         <v>62</v>
       </c>
       <c r="I29" s="34"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="47"/>
-      <c r="L29" s="47"/>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
     </row>
     <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B30" s="22" t="s">
-        <v>86</v>
+      <c r="B30" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C30" s="23">
         <v>27</v>
@@ -3340,32 +3402,32 @@
         <v>1</v>
       </c>
       <c r="E30" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="F30" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="34" t="s">
+      <c r="G30" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="H30" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="I30" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G30" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="H30" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="I30" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="J30" s="50"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
     </row>
     <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="22" t="s">
-        <v>86</v>
+      <c r="B31" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C31" s="23">
         <v>29</v>
@@ -3377,22 +3439,22 @@
         <v>50</v>
       </c>
       <c r="F31" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="H31" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="G31" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="H31" s="34" t="s">
+      <c r="I31" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="I31" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="47"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="46"/>
     </row>
     <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
@@ -3414,17 +3476,17 @@
         <v>43</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H32" s="34" t="s">
         <v>44</v>
       </c>
       <c r="I32" s="34"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="47"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="46"/>
     </row>
     <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
@@ -3454,11 +3516,11 @@
       <c r="I33" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="J33" s="50"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="47"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="46"/>
     </row>
     <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
@@ -3484,20 +3546,20 @@
         <v>7</v>
       </c>
       <c r="I34" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="J34" s="50"/>
-      <c r="K34" s="51"/>
-      <c r="L34" s="51"/>
-      <c r="M34" s="51"/>
-      <c r="N34" s="47"/>
+        <v>160</v>
+      </c>
+      <c r="J34" s="49"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="46"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="22" t="s">
-        <v>86</v>
+      <c r="B35" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C35" s="23">
         <v>33</v>
@@ -3506,25 +3568,25 @@
         <v>1</v>
       </c>
       <c r="E35" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="F35" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="F35" s="34" t="s">
+      <c r="G35" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="G35" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="H35" s="34" t="s">
+      <c r="I35" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="I35" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="J35" s="52"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="47"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="47"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="46"/>
+      <c r="N35" s="46"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
@@ -3549,16 +3611,16 @@
         <v>66</v>
       </c>
       <c r="H36" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I36" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="J36" s="45"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="46"/>
     </row>
     <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
@@ -3577,22 +3639,22 @@
         <v>35</v>
       </c>
       <c r="F37" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="G37" s="34" t="s">
+      <c r="H37" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="H37" s="34" t="s">
+      <c r="I37" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="I37" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="J37" s="50"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="51"/>
-      <c r="M37" s="51"/>
-      <c r="N37" s="47"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="46"/>
     </row>
     <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
@@ -3608,25 +3670,25 @@
         <v>4</v>
       </c>
       <c r="E38" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F38" s="34" t="s">
         <v>39</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H38" s="34" t="s">
         <v>40</v>
       </c>
       <c r="I38" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="J38" s="50"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="47"/>
+        <v>172</v>
+      </c>
+      <c r="J38" s="49"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="46"/>
     </row>
     <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
@@ -3642,25 +3704,25 @@
         <v>8</v>
       </c>
       <c r="E39" s="34" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F39" s="34" t="s">
         <v>20</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H39" s="34">
         <v>805</v>
       </c>
       <c r="I39" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J39" s="50"/>
-      <c r="K39" s="53"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J39" s="49"/>
+      <c r="K39" s="52"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="46"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
@@ -3682,26 +3744,26 @@
         <v>32</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H40" s="34">
         <v>805</v>
       </c>
       <c r="I40" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J40" s="45"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J40" s="44"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
     </row>
     <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="23" t="s">
-        <v>82</v>
+      <c r="B41" s="63" t="s">
+        <v>248</v>
       </c>
       <c r="C41" s="23">
         <v>39</v>
@@ -3713,22 +3775,22 @@
         <v>17</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G41" s="34" t="s">
+        <v>175</v>
+      </c>
+      <c r="H41" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="H41" s="34" t="s">
+      <c r="I41" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="I41" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="J41" s="45"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="47"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="50"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="46"/>
     </row>
     <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
@@ -3744,25 +3806,25 @@
         <v>5</v>
       </c>
       <c r="E42" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F42" s="34" t="s">
         <v>36</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H42" s="34">
         <v>805</v>
       </c>
       <c r="I42" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J42" s="45"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J42" s="44"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="46"/>
     </row>
     <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
@@ -3778,25 +3840,25 @@
         <v>7</v>
       </c>
       <c r="E43" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="F43" s="34" t="s">
-        <v>181</v>
-      </c>
       <c r="G43" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H43" s="34">
         <v>805</v>
       </c>
       <c r="I43" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J43" s="50"/>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
-      <c r="M43" s="51"/>
-      <c r="N43" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J43" s="49"/>
+      <c r="K43" s="50"/>
+      <c r="L43" s="50"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="46"/>
     </row>
     <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
@@ -3812,32 +3874,32 @@
         <v>7</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H44" s="34">
         <v>805</v>
       </c>
       <c r="I44" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J44" s="45"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J44" s="44"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="46"/>
     </row>
     <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="23" t="s">
-        <v>82</v>
+      <c r="B45" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="C45" s="23">
         <v>43</v>
@@ -3846,25 +3908,25 @@
         <v>8</v>
       </c>
       <c r="E45" s="34" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F45" s="34" t="s">
         <v>28</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H45" s="34">
         <v>805</v>
       </c>
       <c r="I45" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J45" s="50"/>
-      <c r="K45" s="53"/>
-      <c r="L45" s="51"/>
-      <c r="M45" s="51"/>
-      <c r="N45" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J45" s="49"/>
+      <c r="K45" s="52"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="46"/>
     </row>
     <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
@@ -3880,32 +3942,32 @@
         <v>6</v>
       </c>
       <c r="E46" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H46" s="34">
         <v>805</v>
       </c>
       <c r="I46" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J46" s="50"/>
-      <c r="K46" s="51"/>
-      <c r="L46" s="51"/>
-      <c r="M46" s="51"/>
-      <c r="N46" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J46" s="49"/>
+      <c r="K46" s="50"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="46"/>
     </row>
     <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="23" t="s">
-        <v>82</v>
+      <c r="B47" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="C47" s="23">
         <v>45</v>
@@ -3914,32 +3976,32 @@
         <v>2</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F47" s="34" t="s">
         <v>23</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H47" s="34">
         <v>805</v>
       </c>
       <c r="I47" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J47" s="45"/>
-      <c r="K47" s="51"/>
-      <c r="L47" s="51"/>
-      <c r="M47" s="51"/>
-      <c r="N47" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J47" s="44"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="46"/>
     </row>
     <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B48" s="23" t="s">
-        <v>82</v>
+      <c r="B48" s="63" t="s">
+        <v>247</v>
       </c>
       <c r="C48" s="23">
         <v>46</v>
@@ -3948,25 +4010,25 @@
         <v>2</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G48" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H48" s="34">
         <v>805</v>
       </c>
       <c r="I48" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J48" s="50"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="51"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J48" s="49"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="50"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="46"/>
     </row>
     <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
@@ -3982,25 +4044,25 @@
         <v>2</v>
       </c>
       <c r="E49" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="F49" s="34" t="s">
         <v>184</v>
       </c>
-      <c r="F49" s="34" t="s">
-        <v>185</v>
-      </c>
       <c r="G49" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H49" s="34">
         <v>805</v>
       </c>
       <c r="I49" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J49" s="50"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="47"/>
-      <c r="M49" s="47"/>
-      <c r="N49" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J49" s="49"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="46"/>
+      <c r="N49" s="46"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
@@ -4022,53 +4084,53 @@
         <v>48</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H50" s="34">
         <v>805</v>
       </c>
       <c r="I50" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J50" s="45"/>
-      <c r="K50" s="46"/>
-      <c r="L50" s="47"/>
-      <c r="M50" s="47"/>
-      <c r="N50" s="47"/>
+        <v>174</v>
+      </c>
+      <c r="J50" s="44"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="46"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>82</v>
+      <c r="A51" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="63" t="s">
+        <v>245</v>
       </c>
       <c r="C51" s="23">
         <v>49</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F51" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G51" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I51" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="J51" s="45"/>
-      <c r="K51" s="54"/>
-      <c r="L51" s="47"/>
-      <c r="M51" s="47"/>
-      <c r="N51" s="47"/>
+        <v>234</v>
+      </c>
+      <c r="J51" s="44"/>
+      <c r="K51" s="53"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="46"/>
+      <c r="N51" s="46"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
@@ -4084,25 +4146,25 @@
         <v>1</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F52" s="34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G52" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H52" s="34">
         <v>805</v>
       </c>
       <c r="I52" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J52" s="55"/>
-      <c r="K52" s="55"/>
-      <c r="L52" s="56"/>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J52" s="54"/>
+      <c r="K52" s="54"/>
+      <c r="L52" s="55"/>
+      <c r="M52" s="55"/>
+      <c r="N52" s="55"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
@@ -4121,22 +4183,22 @@
         <v>41</v>
       </c>
       <c r="F53" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H53" s="34">
         <v>805</v>
       </c>
       <c r="I53" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J53" s="55"/>
-      <c r="K53" s="56"/>
-      <c r="L53" s="56"/>
-      <c r="M53" s="56"/>
-      <c r="N53" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J53" s="54"/>
+      <c r="K53" s="55"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="55"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
@@ -4152,25 +4214,25 @@
         <v>2</v>
       </c>
       <c r="E54" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F54" s="34" t="s">
         <v>95</v>
       </c>
       <c r="G54" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H54" s="34">
         <v>805</v>
       </c>
       <c r="I54" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J54" s="55"/>
-      <c r="K54" s="56"/>
-      <c r="L54" s="56"/>
-      <c r="M54" s="56"/>
-      <c r="N54" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J54" s="54"/>
+      <c r="K54" s="55"/>
+      <c r="L54" s="55"/>
+      <c r="M54" s="55"/>
+      <c r="N54" s="55"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
@@ -4192,19 +4254,19 @@
         <v>37</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H55" s="34">
         <v>805</v>
       </c>
       <c r="I55" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J55" s="55"/>
-      <c r="K55" s="56"/>
-      <c r="L55" s="56"/>
-      <c r="M55" s="56"/>
-      <c r="N55" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J55" s="54"/>
+      <c r="K55" s="55"/>
+      <c r="L55" s="55"/>
+      <c r="M55" s="55"/>
+      <c r="N55" s="55"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
@@ -4226,19 +4288,19 @@
         <v>97</v>
       </c>
       <c r="G56" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H56" s="34">
         <v>805</v>
       </c>
       <c r="I56" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J56" s="57"/>
-      <c r="K56" s="56"/>
-      <c r="L56" s="56"/>
-      <c r="M56" s="56"/>
-      <c r="N56" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J56" s="56"/>
+      <c r="K56" s="55"/>
+      <c r="L56" s="55"/>
+      <c r="M56" s="55"/>
+      <c r="N56" s="55"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
@@ -4254,25 +4316,25 @@
         <v>1</v>
       </c>
       <c r="E57" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F57" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H57" s="34">
         <v>805</v>
       </c>
       <c r="I57" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J57" s="57"/>
-      <c r="K57" s="56"/>
-      <c r="L57" s="56"/>
-      <c r="M57" s="56"/>
-      <c r="N57" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J57" s="56"/>
+      <c r="K57" s="55"/>
+      <c r="L57" s="55"/>
+      <c r="M57" s="55"/>
+      <c r="N57" s="55"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
@@ -4288,59 +4350,59 @@
         <v>2</v>
       </c>
       <c r="E58" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F58" s="34" t="s">
         <v>98</v>
       </c>
       <c r="G58" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H58" s="34">
         <v>805</v>
       </c>
       <c r="I58" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J58" s="57"/>
-      <c r="K58" s="58"/>
-      <c r="L58" s="56"/>
-      <c r="M58" s="56"/>
-      <c r="N58" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J58" s="56"/>
+      <c r="K58" s="57"/>
+      <c r="L58" s="55"/>
+      <c r="M58" s="55"/>
+      <c r="N58" s="55"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A59" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B59" s="23" t="s">
-        <v>82</v>
+      <c r="A59" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="63" t="s">
+        <v>245</v>
       </c>
       <c r="C59" s="23">
         <v>57</v>
       </c>
       <c r="D59" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E59" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F59" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H59" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I59" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="J59" s="57"/>
-      <c r="K59" s="56"/>
-      <c r="L59" s="56"/>
-      <c r="M59" s="56"/>
-      <c r="N59" s="56"/>
+        <v>234</v>
+      </c>
+      <c r="J59" s="56"/>
+      <c r="K59" s="55"/>
+      <c r="L59" s="55"/>
+      <c r="M59" s="55"/>
+      <c r="N59" s="55"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
@@ -4362,19 +4424,19 @@
         <v>29</v>
       </c>
       <c r="G60" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H60" s="34">
         <v>805</v>
       </c>
       <c r="I60" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J60" s="57"/>
-      <c r="K60" s="56"/>
-      <c r="L60" s="56"/>
-      <c r="M60" s="56"/>
-      <c r="N60" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J60" s="56"/>
+      <c r="K60" s="55"/>
+      <c r="L60" s="55"/>
+      <c r="M60" s="55"/>
+      <c r="N60" s="55"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
@@ -4396,19 +4458,19 @@
         <v>100</v>
       </c>
       <c r="G61" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H61" s="34">
         <v>805</v>
       </c>
       <c r="I61" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J61" s="57"/>
-      <c r="K61" s="56"/>
-      <c r="L61" s="56"/>
-      <c r="M61" s="56"/>
-      <c r="N61" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J61" s="56"/>
+      <c r="K61" s="55"/>
+      <c r="L61" s="55"/>
+      <c r="M61" s="55"/>
+      <c r="N61" s="55"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
@@ -4430,19 +4492,19 @@
         <v>26</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H62" s="34">
         <v>805</v>
       </c>
       <c r="I62" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J62" s="57"/>
-      <c r="K62" s="56"/>
-      <c r="L62" s="56"/>
-      <c r="M62" s="56"/>
-      <c r="N62" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J62" s="56"/>
+      <c r="K62" s="55"/>
+      <c r="L62" s="55"/>
+      <c r="M62" s="55"/>
+      <c r="N62" s="55"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
@@ -4464,19 +4526,19 @@
         <v>53</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H63" s="34">
         <v>805</v>
       </c>
       <c r="I63" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J63" s="57"/>
-      <c r="K63" s="56"/>
-      <c r="L63" s="56"/>
-      <c r="M63" s="56"/>
-      <c r="N63" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J63" s="56"/>
+      <c r="K63" s="55"/>
+      <c r="L63" s="55"/>
+      <c r="M63" s="55"/>
+      <c r="N63" s="55"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
@@ -4498,19 +4560,19 @@
         <v>46</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H64" s="34">
         <v>805</v>
       </c>
       <c r="I64" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J64" s="57"/>
-      <c r="K64" s="58"/>
-      <c r="L64" s="56"/>
-      <c r="M64" s="56"/>
-      <c r="N64" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J64" s="56"/>
+      <c r="K64" s="57"/>
+      <c r="L64" s="55"/>
+      <c r="M64" s="55"/>
+      <c r="N64" s="55"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
@@ -4526,25 +4588,25 @@
         <v>1</v>
       </c>
       <c r="E65" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="F65" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="F65" s="34" t="s">
-        <v>219</v>
-      </c>
       <c r="G65" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H65" s="34">
         <v>805</v>
       </c>
       <c r="I65" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J65" s="57"/>
-      <c r="K65" s="58"/>
-      <c r="L65" s="56"/>
-      <c r="M65" s="56"/>
-      <c r="N65" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J65" s="56"/>
+      <c r="K65" s="57"/>
+      <c r="L65" s="55"/>
+      <c r="M65" s="55"/>
+      <c r="N65" s="55"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
@@ -4560,25 +4622,25 @@
         <v>1</v>
       </c>
       <c r="E66" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F66" s="34" t="s">
         <v>101</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H66" s="34">
         <v>1206</v>
       </c>
       <c r="I66" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J66" s="55"/>
-      <c r="K66" s="58"/>
-      <c r="L66" s="56"/>
-      <c r="M66" s="56"/>
-      <c r="N66" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J66" s="54"/>
+      <c r="K66" s="57"/>
+      <c r="L66" s="55"/>
+      <c r="M66" s="55"/>
+      <c r="N66" s="55"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
@@ -4608,11 +4670,11 @@
       <c r="I67" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="J67" s="55"/>
-      <c r="K67" s="58"/>
-      <c r="L67" s="56"/>
-      <c r="M67" s="56"/>
-      <c r="N67" s="56"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="57"/>
+      <c r="L67" s="55"/>
+      <c r="M67" s="55"/>
+      <c r="N67" s="55"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="22" t="s">
@@ -4640,11 +4702,11 @@
       <c r="I68" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="J68" s="55"/>
-      <c r="K68" s="56"/>
-      <c r="L68" s="56"/>
-      <c r="M68" s="56"/>
-      <c r="N68" s="56"/>
+      <c r="J68" s="54"/>
+      <c r="K68" s="55"/>
+      <c r="L68" s="55"/>
+      <c r="M68" s="55"/>
+      <c r="N68" s="55"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="22" t="s">
@@ -4663,22 +4725,22 @@
         <v>55</v>
       </c>
       <c r="F69" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="G69" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="H69" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="I69" s="34" t="s">
         <v>193</v>
       </c>
-      <c r="G69" s="34" t="s">
-        <v>193</v>
-      </c>
-      <c r="H69" s="34" t="s">
-        <v>193</v>
-      </c>
-      <c r="I69" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="J69" s="55"/>
-      <c r="K69" s="56"/>
-      <c r="L69" s="56"/>
-      <c r="M69" s="56"/>
-      <c r="N69" s="56"/>
+      <c r="J69" s="54"/>
+      <c r="K69" s="55"/>
+      <c r="L69" s="55"/>
+      <c r="M69" s="55"/>
+      <c r="N69" s="55"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="22" t="s">
@@ -4706,20 +4768,20 @@
         <v>109</v>
       </c>
       <c r="I70" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="J70" s="55"/>
-      <c r="K70" s="56"/>
-      <c r="L70" s="56"/>
-      <c r="M70" s="56"/>
-      <c r="N70" s="56"/>
+        <v>194</v>
+      </c>
+      <c r="J70" s="54"/>
+      <c r="K70" s="55"/>
+      <c r="L70" s="55"/>
+      <c r="M70" s="55"/>
+      <c r="N70" s="55"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B71" s="22" t="s">
-        <v>86</v>
+      <c r="B71" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C71" s="23">
         <v>69</v>
@@ -4728,32 +4790,32 @@
         <v>1</v>
       </c>
       <c r="E71" s="34" t="s">
+        <v>195</v>
+      </c>
+      <c r="F71" s="34" t="s">
         <v>196</v>
       </c>
-      <c r="F71" s="34" t="s">
+      <c r="G71" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="G71" s="34" t="s">
+      <c r="H71" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="H71" s="34" t="s">
+      <c r="I71" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="I71" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="J71" s="55"/>
-      <c r="K71" s="56"/>
-      <c r="L71" s="56"/>
-      <c r="M71" s="56"/>
-      <c r="N71" s="56"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="55"/>
+      <c r="L71" s="55"/>
+      <c r="M71" s="55"/>
+      <c r="N71" s="55"/>
     </row>
     <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="22" t="s">
-        <v>86</v>
+      <c r="B72" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C72" s="23">
         <v>70</v>
@@ -4762,32 +4824,32 @@
         <v>1</v>
       </c>
       <c r="E72" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="F72" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="F72" s="34" t="s">
+      <c r="G72" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="H72" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="G72" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="H72" s="34" t="s">
+      <c r="I72" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="I72" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="J72" s="59"/>
-      <c r="K72" s="51"/>
-      <c r="L72" s="51"/>
-      <c r="M72" s="51"/>
-      <c r="N72" s="47"/>
+      <c r="J72" s="58"/>
+      <c r="K72" s="50"/>
+      <c r="L72" s="50"/>
+      <c r="M72" s="50"/>
+      <c r="N72" s="46"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B73" s="22" t="s">
-        <v>86</v>
+      <c r="A73" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C73" s="23">
         <v>71</v>
@@ -4799,29 +4861,29 @@
         <v>6</v>
       </c>
       <c r="F73" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="G73" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="G73" s="34" t="s">
+      <c r="H73" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="H73" s="34" t="s">
+      <c r="I73" s="34" t="s">
         <v>207</v>
       </c>
-      <c r="I73" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="J73" s="55"/>
-      <c r="K73" s="56"/>
-      <c r="L73" s="56"/>
-      <c r="M73" s="56"/>
-      <c r="N73" s="56"/>
+      <c r="J73" s="54"/>
+      <c r="K73" s="55"/>
+      <c r="L73" s="55"/>
+      <c r="M73" s="55"/>
+      <c r="N73" s="55"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B74" s="22" t="s">
-        <v>86</v>
+      <c r="B74" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C74" s="23">
         <v>72</v>
@@ -4833,22 +4895,22 @@
         <v>51</v>
       </c>
       <c r="F74" s="34" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G74" s="34">
         <v>7414</v>
       </c>
       <c r="H74" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I74" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="J74" s="56"/>
-      <c r="K74" s="56"/>
-      <c r="L74" s="56"/>
-      <c r="M74" s="56"/>
-      <c r="N74" s="56"/>
+      <c r="J74" s="55"/>
+      <c r="K74" s="55"/>
+      <c r="L74" s="55"/>
+      <c r="M74" s="55"/>
+      <c r="N74" s="55"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="22" t="s">
@@ -4867,29 +4929,29 @@
         <v>69</v>
       </c>
       <c r="F75" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="G75" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="H75" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="G75" s="34" t="s">
+      <c r="I75" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="H75" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="I75" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="J75" s="56"/>
-      <c r="K75" s="56"/>
-      <c r="L75" s="56"/>
-      <c r="M75" s="56"/>
-      <c r="N75" s="56"/>
+      <c r="J75" s="55"/>
+      <c r="K75" s="55"/>
+      <c r="L75" s="55"/>
+      <c r="M75" s="55"/>
+      <c r="N75" s="55"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B76" s="22" t="s">
-        <v>86</v>
+      <c r="B76" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C76" s="23">
         <v>74</v>
@@ -4901,22 +4963,22 @@
         <v>65</v>
       </c>
       <c r="F76" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="G76" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="H76" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="G76" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="H76" s="34" t="s">
+      <c r="I76" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="I76" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="J76" s="55"/>
-      <c r="K76" s="56"/>
-      <c r="L76" s="56"/>
-      <c r="M76" s="56"/>
-      <c r="N76" s="56"/>
+      <c r="J76" s="54"/>
+      <c r="K76" s="55"/>
+      <c r="L76" s="55"/>
+      <c r="M76" s="55"/>
+      <c r="N76" s="55"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
@@ -4944,18 +5006,18 @@
         <v>14</v>
       </c>
       <c r="I77" s="34"/>
-      <c r="J77" s="55"/>
-      <c r="K77" s="56"/>
-      <c r="L77" s="56"/>
-      <c r="M77" s="56"/>
-      <c r="N77" s="56"/>
+      <c r="J77" s="54"/>
+      <c r="K77" s="55"/>
+      <c r="L77" s="55"/>
+      <c r="M77" s="55"/>
+      <c r="N77" s="55"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B78" s="22" t="s">
-        <v>86</v>
+      <c r="B78" s="63" t="s">
+        <v>248</v>
       </c>
       <c r="C78" s="23">
         <v>76</v>
@@ -4967,22 +5029,22 @@
         <v>16</v>
       </c>
       <c r="F78" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="G78" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="H78" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="I78" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="G78" s="34" t="s">
-        <v>237</v>
-      </c>
-      <c r="H78" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="I78" s="34" t="s">
-        <v>239</v>
-      </c>
-      <c r="J78" s="55"/>
-      <c r="K78" s="56"/>
-      <c r="L78" s="56"/>
-      <c r="M78" s="56"/>
-      <c r="N78" s="56"/>
+      <c r="J78" s="54"/>
+      <c r="K78" s="55"/>
+      <c r="L78" s="55"/>
+      <c r="M78" s="55"/>
+      <c r="N78" s="55"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
@@ -5010,18 +5072,18 @@
         <v>107</v>
       </c>
       <c r="I79" s="34"/>
-      <c r="J79" s="55"/>
-      <c r="K79" s="56"/>
-      <c r="L79" s="56"/>
-      <c r="M79" s="56"/>
-      <c r="N79" s="56"/>
+      <c r="J79" s="54"/>
+      <c r="K79" s="55"/>
+      <c r="L79" s="55"/>
+      <c r="M79" s="55"/>
+      <c r="N79" s="55"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="22" t="s">
-        <v>86</v>
+      <c r="B80" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="C80" s="23">
         <v>78</v>
@@ -5033,29 +5095,29 @@
         <v>25</v>
       </c>
       <c r="F80" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="G80" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="H80" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="G80" s="34" t="s">
-        <v>214</v>
-      </c>
-      <c r="H80" s="34" t="s">
+      <c r="I80" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="I80" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="J80" s="55"/>
-      <c r="K80" s="56"/>
-      <c r="L80" s="56"/>
-      <c r="M80" s="56"/>
-      <c r="N80" s="56"/>
+      <c r="J80" s="54"/>
+      <c r="K80" s="55"/>
+      <c r="L80" s="55"/>
+      <c r="M80" s="55"/>
+      <c r="N80" s="55"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B81" s="22" t="s">
-        <v>86</v>
+      <c r="B81" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="C81" s="23">
         <v>79</v>
@@ -5063,33 +5125,33 @@
       <c r="D81" s="34">
         <v>1</v>
       </c>
-      <c r="E81" s="60" t="s">
-        <v>226</v>
-      </c>
-      <c r="F81" s="63">
+      <c r="E81" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="F81" s="61">
         <v>0</v>
       </c>
-      <c r="G81" s="61" t="s">
-        <v>174</v>
+      <c r="G81" s="34" t="s">
+        <v>173</v>
       </c>
       <c r="H81" s="34">
         <v>805</v>
       </c>
       <c r="I81" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J81" s="55"/>
-      <c r="K81" s="56"/>
-      <c r="L81" s="56"/>
-      <c r="M81" s="56"/>
-      <c r="N81" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J81" s="54"/>
+      <c r="K81" s="55"/>
+      <c r="L81" s="55"/>
+      <c r="M81" s="55"/>
+      <c r="N81" s="55"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="22" t="s">
-        <v>86</v>
+      <c r="B82" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="C82" s="23">
         <v>80</v>
@@ -5097,11 +5159,11 @@
       <c r="D82" s="34">
         <v>1</v>
       </c>
-      <c r="E82" s="60" t="s">
-        <v>229</v>
+      <c r="E82" s="59" t="s">
+        <v>227</v>
       </c>
       <c r="F82" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G82" s="34" t="s">
         <v>56</v>
@@ -5112,18 +5174,18 @@
       <c r="I82" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="J82" s="55"/>
-      <c r="K82" s="56"/>
-      <c r="L82" s="56"/>
-      <c r="M82" s="56"/>
-      <c r="N82" s="56"/>
+      <c r="J82" s="54"/>
+      <c r="K82" s="55"/>
+      <c r="L82" s="55"/>
+      <c r="M82" s="55"/>
+      <c r="N82" s="55"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="22" t="s">
-        <v>86</v>
+      <c r="B83" s="63" t="s">
+        <v>246</v>
       </c>
       <c r="C83" s="23">
         <v>81</v>
@@ -5132,89 +5194,114 @@
         <v>1</v>
       </c>
       <c r="E83" s="34" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F83" s="34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G83" s="34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H83" s="34">
         <v>805</v>
       </c>
       <c r="I83" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="J83" s="55"/>
-      <c r="K83" s="56"/>
-      <c r="L83" s="56"/>
-      <c r="M83" s="56"/>
-      <c r="N83" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="J83" s="54"/>
+      <c r="K83" s="55"/>
+      <c r="L83" s="55"/>
+      <c r="M83" s="55"/>
+      <c r="N83" s="55"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="H84" s="64"/>
+      <c r="H84" s="62"/>
     </row>
   </sheetData>
   <phoneticPr fontId="48" type="noConversion"/>
   <conditionalFormatting sqref="A66:A70">
-    <cfRule type="containsText" dxfId="15" priority="32" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="20" priority="46" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",A66)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:B80">
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="P">
+  <conditionalFormatting sqref="A7:A8 A74:A81 A60:A72 A52:A58 A10:A50 B41 B45 B47:B48 B51 B59 B78 B81:B83">
+    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",A7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",B29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
-    <cfRule type="containsText" dxfId="11" priority="24" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",B67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",B70)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A81:B81">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="P">
-      <formula>NOT(ISERROR(SEARCH("P",A81)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",A81)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82:B83">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="P">
-      <formula>NOT(ISERROR(SEARCH("P",B82)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",B82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A82">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A82)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",A82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A83">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",A83)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",A83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A73">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A73)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",A73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A59">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A59)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",A59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A51)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",A51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",A9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",A9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:B40">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",B7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",B7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B42:B44">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",B42)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",B42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79:B80 B60:B77 B52:B58 B49:B50 B46">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",B46)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",A83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NO",B46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5226,8 +5313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5261,50 +5348,58 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="38">
+        <v>45020</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="B4" s="39">
-        <v>45020</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>221</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="5" spans="1:4" ht="102" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="B5" s="42">
+      <c r="A5" s="40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="41">
         <v>45076</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>246</v>
+      <c r="C5" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="26"/>
+      <c r="A6" s="40">
+        <v>3</v>
+      </c>
+      <c r="B6" s="41">
+        <v>45077</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
-      <c r="B7" s="42"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>

</xml_diff>